<commit_message>
Added changes on 23/07/2018
</commit_message>
<xml_diff>
--- a/Customers/NextGen/TestSuite1.xlsx
+++ b/Customers/NextGen/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19695" windowHeight="11025" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19695" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,11 @@
     <sheet name="TC06" sheetId="15" r:id="rId7"/>
     <sheet name="TC07" sheetId="16" r:id="rId8"/>
     <sheet name="TC08" sheetId="11" r:id="rId9"/>
-    <sheet name="TC09" sheetId="18" r:id="rId10"/>
+    <sheet name="TC09" sheetId="24" r:id="rId10"/>
     <sheet name="TC10" sheetId="20" r:id="rId11"/>
     <sheet name="TC11" sheetId="21" r:id="rId12"/>
     <sheet name="TC12" sheetId="22" r:id="rId13"/>
+    <sheet name="TC13" sheetId="23" r:id="rId14"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2194" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="355">
   <si>
     <t>TCID</t>
   </si>
@@ -465,9 +466,6 @@
     <t>CPARTitle</t>
   </si>
   <si>
-    <t>Waiting for Charges/Payments/Adjustments/Refunds widget title</t>
-  </si>
-  <si>
     <t>Verify Charges, payments, adjustments, refunds widget title</t>
   </si>
   <si>
@@ -927,9 +925,6 @@
     <t>Close change password dialog</t>
   </si>
   <si>
-    <t>Waiting for Run as label</t>
-  </si>
-  <si>
     <t>FilterLabel</t>
   </si>
   <si>
@@ -1087,6 +1082,24 @@
   </si>
   <si>
     <t>wait for pop up</t>
+  </si>
+  <si>
+    <t>TC13</t>
+  </si>
+  <si>
+    <t>Manage widgets</t>
+  </si>
+  <si>
+    <t>Waiting for page ready state</t>
+  </si>
+  <si>
+    <t>waitForPageReadyState</t>
+  </si>
+  <si>
+    <t>clickWhenReady</t>
+  </si>
+  <si>
+    <t>Waiting for filter icon</t>
   </si>
 </sst>
 </file>
@@ -1464,10 +1477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1536,7 +1549,7 @@
         <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
         <v>82</v>
@@ -1547,7 +1560,7 @@
         <v>140</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
         <v>82</v>
@@ -1555,10 +1568,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
@@ -1566,7 +1579,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
@@ -1577,10 +1590,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C10" t="s">
         <v>82</v>
@@ -1588,10 +1601,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C11" t="s">
         <v>82</v>
@@ -1599,10 +1612,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -1610,12 +1623,23 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>349</v>
+      </c>
+      <c r="B14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1626,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1679,73 +1703,74 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -1754,13 +1779,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
@@ -1772,51 +1797,51 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>281</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
         <v>283</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1825,16 +1850,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -1843,141 +1868,143 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>288</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>289</v>
+        <v>133</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>133</v>
+        <v>291</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>290</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>133</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>291</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>292</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>293</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>22</v>
+      <c r="F18" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>294</v>
@@ -1985,57 +2012,54 @@
       <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
-        <v>294</v>
-      </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>296</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" t="s">
-        <v>295</v>
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
-      </c>
-      <c r="F21" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -2043,50 +2067,50 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>46</v>
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
-      </c>
-      <c r="F24" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
@@ -2094,13 +2118,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
         <v>29</v>
@@ -2108,59 +2132,60 @@
       <c r="E26" t="s">
         <v>4</v>
       </c>
+      <c r="F26" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>28</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>290</v>
-      </c>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -2169,13 +2194,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
         <v>45</v>
@@ -2187,51 +2212,51 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>22</v>
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>281</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
         <v>283</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -2240,16 +2265,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -2258,41 +2283,41 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="4" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>186</v>
       </c>
       <c r="B36" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>290</v>
-      </c>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
@@ -2302,34 +2327,33 @@
         <v>288</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E37" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>188</v>
       </c>
       <c r="B38" t="s">
-        <v>289</v>
+        <v>133</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
       <c r="E38" t="s">
         <v>4</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2337,51 +2361,54 @@
         <v>189</v>
       </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>291</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>290</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="B40" t="s">
-        <v>292</v>
+        <v>133</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" t="s">
-        <v>291</v>
+        <v>22</v>
       </c>
       <c r="E40" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>235</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>292</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="D41" t="s">
+        <v>293</v>
       </c>
       <c r="E41" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>22</v>
+      <c r="F41" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2389,10 +2416,10 @@
         <v>236</v>
       </c>
       <c r="B42" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
         <v>294</v>
@@ -2400,57 +2427,55 @@
       <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="F42" t="s">
-        <v>294</v>
-      </c>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>237</v>
       </c>
       <c r="B43" t="s">
-        <v>296</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
-        <v>295</v>
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="4"/>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>238</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
       </c>
       <c r="E44" t="s">
         <v>4</v>
       </c>
-      <c r="F44" t="s">
-        <v>22</v>
-      </c>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E45" t="s">
         <v>4</v>
@@ -2462,34 +2487,33 @@
         <v>264</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" t="s">
-        <v>46</v>
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>22</v>
       </c>
       <c r="E46" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="4"/>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>265</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
       </c>
       <c r="E47" t="s">
         <v>4</v>
-      </c>
-      <c r="F47" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2497,32 +2521,15 @@
         <v>266</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>267</v>
-      </c>
-      <c r="B49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" t="s">
-        <v>29</v>
-      </c>
-      <c r="E49" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2536,10 +2543,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:F22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2652,10 +2659,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>78</v>
+        <v>353</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -2670,13 +2677,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>129</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>16</v>
+        <v>353</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -2688,55 +2695,53 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>16</v>
+        <v>353</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>130</v>
+        <v>353</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2744,31 +2749,30 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>354</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>301</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>302</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>16</v>
+        <v>353</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>301</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -2779,16 +2783,16 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>57</v>
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2796,16 +2800,19 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
+        <v>305</v>
+      </c>
+      <c r="C14" t="s">
+        <v>307</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>303</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2813,16 +2820,19 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
+        <v>306</v>
+      </c>
+      <c r="C15" t="s">
+        <v>307</v>
+      </c>
+      <c r="D15" t="s">
         <v>304</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>303</v>
-      </c>
       <c r="E15" t="s">
         <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2830,16 +2840,16 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2847,19 +2857,16 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
-      </c>
-      <c r="C17" t="s">
-        <v>309</v>
-      </c>
-      <c r="D17" t="s">
-        <v>305</v>
+        <v>133</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
-        <v>310</v>
+      <c r="F17" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2867,19 +2874,16 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
-      </c>
-      <c r="C18" t="s">
-        <v>309</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>306</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2887,67 +2891,13 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" t="s">
         <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2962,7 +2912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -3005,7 +2955,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -3250,13 +3200,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -3284,13 +3234,13 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -3301,19 +3251,19 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3321,13 +3271,13 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
@@ -3338,13 +3288,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -3355,13 +3305,13 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -3389,13 +3339,13 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C24" t="s">
         <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -3406,16 +3356,16 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
+        <v>338</v>
+      </c>
+      <c r="F25" t="s">
         <v>340</v>
-      </c>
-      <c r="F25" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3423,19 +3373,19 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3443,13 +3393,13 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -3477,7 +3427,7 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>16</v>
@@ -3494,13 +3444,13 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
+        <v>334</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
         <v>336</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>338</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
@@ -3511,13 +3461,13 @@
         <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -3528,13 +3478,13 @@
         <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -3562,13 +3512,13 @@
         <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C34" t="s">
         <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -3579,50 +3529,50 @@
         <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F35" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E37" t="s">
         <v>4</v>
@@ -3633,7 +3583,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" t="s">
         <v>22</v>
@@ -3647,10 +3597,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>16</v>
@@ -3664,16 +3614,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B40" t="s">
+        <v>343</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s">
         <v>345</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" t="s">
-        <v>347</v>
       </c>
       <c r="E40" t="s">
         <v>4</v>
@@ -3681,16 +3631,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B41" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E41" t="s">
         <v>4</v>
@@ -3698,7 +3648,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B42" t="s">
         <v>133</v>
@@ -3715,16 +3665,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B43" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D43" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
@@ -3733,7 +3683,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
@@ -3750,7 +3700,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B45" t="s">
         <v>133</v>
@@ -3767,7 +3717,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -3784,7 +3734,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -3853,7 +3803,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -4101,13 +4051,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -4135,16 +4085,339 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
+        <v>329</v>
+      </c>
+      <c r="C18" t="s">
         <v>331</v>
       </c>
-      <c r="C18" t="s">
-        <v>333</v>
-      </c>
       <c r="D18" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4292,7 +4565,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -4366,7 +4639,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4605,13 +4878,10 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>297</v>
+        <v>351</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>298</v>
+        <v>352</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -4622,16 +4892,16 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4889,7 +5159,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5180,13 +5450,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>351</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>88</v>
+        <v>352</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -5546,7 +5813,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5837,13 +6104,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>351</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>142</v>
+        <v>352</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -5854,7 +6118,7 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
@@ -5880,7 +6144,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -5908,19 +6172,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -5928,13 +6192,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
         <v>148</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>149</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -5945,19 +6209,19 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5971,7 +6235,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -5999,19 +6263,19 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6019,13 +6283,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
         <v>154</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" t="s">
-        <v>155</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -6036,19 +6300,19 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -6062,7 +6326,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -6090,19 +6354,19 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6202,8 +6466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6494,13 +6758,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -6511,19 +6775,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6537,7 +6801,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -6565,19 +6829,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6602,13 +6866,13 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -6619,19 +6883,19 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -6645,7 +6909,7 @@
         <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -6673,19 +6937,19 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -6693,13 +6957,13 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -6710,19 +6974,19 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -6736,7 +7000,7 @@
         <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -6764,19 +7028,19 @@
         <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6784,13 +7048,13 @@
         <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -6801,19 +7065,19 @@
         <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -6827,7 +7091,7 @@
         <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -6852,24 +7116,24 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -6886,7 +7150,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -6903,7 +7167,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
         <v>108</v>
@@ -6920,7 +7184,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
@@ -6937,7 +7201,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B41" t="s">
         <v>124</v>
@@ -6964,7 +7228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -7255,13 +7519,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -7272,19 +7536,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7298,7 +7562,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -7309,19 +7573,19 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -7346,13 +7610,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -7363,19 +7627,19 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -7389,7 +7653,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -7417,19 +7681,19 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -7437,13 +7701,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -7454,19 +7718,19 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7480,7 +7744,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -7508,19 +7772,19 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -7528,13 +7792,13 @@
         <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -7545,19 +7809,19 @@
         <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -7571,7 +7835,7 @@
         <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -7599,21 +7863,21 @@
         <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -7630,7 +7894,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -7647,7 +7911,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" t="s">
         <v>108</v>
@@ -7664,7 +7928,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
         <v>36</v>
@@ -7681,7 +7945,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B40" t="s">
         <v>124</v>
@@ -7708,8 +7972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7999,13 +8263,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -8016,19 +8280,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -8042,7 +8306,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -8070,19 +8334,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -8090,13 +8354,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -8107,19 +8371,19 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -8133,7 +8397,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -8161,19 +8425,19 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -8181,13 +8445,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -8198,19 +8462,19 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -8224,7 +8488,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -8252,19 +8516,19 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -8272,13 +8536,13 @@
         <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -8289,19 +8553,19 @@
         <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -8315,7 +8579,7 @@
         <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -8343,33 +8607,33 @@
         <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
@@ -8377,27 +8641,27 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E37" t="s">
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B38" t="s">
         <v>77</v>
@@ -8406,7 +8670,7 @@
         <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E38" t="s">
         <v>4</v>
@@ -8414,7 +8678,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B39" t="s">
         <v>108</v>
@@ -8431,36 +8695,36 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E40" t="s">
         <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E41" t="s">
         <v>4</v>
@@ -8468,27 +8732,27 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E42" t="s">
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B43" t="s">
         <v>77</v>
@@ -8497,7 +8761,7 @@
         <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
@@ -8505,7 +8769,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B44" t="s">
         <v>108</v>
@@ -8522,36 +8786,36 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E45" t="s">
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E46" t="s">
         <v>4</v>
@@ -8559,27 +8823,27 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E47" t="s">
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B48" t="s">
         <v>77</v>
@@ -8588,7 +8852,7 @@
         <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E48" t="s">
         <v>4</v>
@@ -8596,7 +8860,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B49" t="s">
         <v>108</v>
@@ -8613,27 +8877,27 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E50" t="s">
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B51" t="s">
         <v>35</v>
@@ -8650,7 +8914,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -8667,7 +8931,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B53" t="s">
         <v>108</v>
@@ -8684,7 +8948,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B54" t="s">
         <v>36</v>
@@ -8701,7 +8965,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B55" t="s">
         <v>124</v>
@@ -8729,7 +8993,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:E20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9002,7 +9266,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>78</v>
@@ -9019,10 +9283,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D16" t="s">
         <v>111</v>
@@ -9050,7 +9314,7 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>16</v>
@@ -9149,10 +9413,10 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D24" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
fixed view data as
</commit_message>
<xml_diff>
--- a/Customers/NextGen/TestSuite1.xlsx
+++ b/Customers/NextGen/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19695" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19695" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2473" uniqueCount="368">
   <si>
     <t>TCID</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Wait for remove page from link</t>
   </si>
   <si>
-    <t>https://test.wshcloud.com/</t>
-  </si>
-  <si>
     <t>Homepage_DailyVisitsBillsTitleMenu</t>
   </si>
   <si>
@@ -407,9 +404,6 @@
     <t>VerifyRevenueAnalyticsMenus</t>
   </si>
   <si>
-    <t>https://nextgen.wshcloud.com/</t>
-  </si>
-  <si>
     <t>Waiting for user name text box</t>
   </si>
   <si>
@@ -1010,9 +1004,6 @@
     <t>PracticeFilterValues</t>
   </si>
   <si>
-    <t>https://uat.wshcloud.com/</t>
-  </si>
-  <si>
     <t>DailyVisitsBillsFullscreen</t>
   </si>
   <si>
@@ -1140,6 +1131,15 @@
   </si>
   <si>
     <t>dragAndDrop</t>
+  </si>
+  <si>
+    <t>https://alpha.wshcloud.com/</t>
+  </si>
+  <si>
+    <t>RunAsSearch</t>
+  </si>
+  <si>
+    <t>Click on vew as drop down button</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1207,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -1215,6 +1215,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1519,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1556,10 +1557,10 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1578,7 +1579,7 @@
         <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
@@ -1589,7 +1590,7 @@
         <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>82</v>
@@ -1597,10 +1598,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
         <v>82</v>
@@ -1608,10 +1609,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
@@ -1619,7 +1620,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
@@ -1630,10 +1631,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C10" t="s">
         <v>82</v>
@@ -1641,10 +1642,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C11" t="s">
         <v>82</v>
@@ -1652,21 +1653,21 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C13" t="s">
         <v>82</v>
@@ -1674,10 +1675,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B14" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C14" t="s">
         <v>82</v>
@@ -1692,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1734,7 +1735,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>119</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -1804,7 +1805,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>78</v>
@@ -1840,7 +1841,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>22</v>
@@ -1857,13 +1858,13 @@
         <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -1875,13 +1876,13 @@
         <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -1893,13 +1894,13 @@
         <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -1911,13 +1912,13 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -1931,13 +1932,13 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
         <v>287</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>289</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -1949,19 +1950,19 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1969,7 +1970,7 @@
         <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>22</v>
@@ -1986,13 +1987,13 @@
         <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -2004,7 +2005,7 @@
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>22</v>
@@ -2021,19 +2022,19 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2041,13 +2042,13 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
@@ -2193,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2219,7 +2220,7 @@
         <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>78</v>
@@ -2234,7 +2235,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
@@ -2252,10 +2253,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>22</v>
@@ -2269,16 +2270,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -2287,16 +2288,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -2305,16 +2306,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -2323,36 +2324,36 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B35" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B36" t="s">
+        <v>285</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
         <v>287</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" t="s">
-        <v>289</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
@@ -2361,16 +2362,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E37" t="s">
         <v>4</v>
@@ -2381,10 +2382,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>22</v>
@@ -2398,16 +2399,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B39" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
@@ -2416,10 +2417,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>22</v>
@@ -2433,36 +2434,36 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B41" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E41" t="s">
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E42" t="s">
         <v>4</v>
@@ -2471,7 +2472,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B43" t="s">
         <v>108</v>
@@ -2488,7 +2489,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
@@ -2506,7 +2507,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B45" t="s">
         <v>24</v>
@@ -2524,7 +2525,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B46" t="s">
         <v>108</v>
@@ -2541,7 +2542,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B47" t="s">
         <v>36</v>
@@ -2558,7 +2559,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -2574,9 +2575,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2586,7 +2584,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2629,7 +2627,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -2702,7 +2700,7 @@
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -2717,13 +2715,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -2735,19 +2733,19 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2758,7 +2756,7 @@
         <v>55</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D9" t="s">
         <v>44</v>
@@ -2775,7 +2773,7 @@
         <v>86</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D10" t="s">
         <v>57</v>
@@ -2789,13 +2787,13 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -2806,13 +2804,13 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -2840,19 +2838,19 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" t="s">
         <v>305</v>
       </c>
-      <c r="C14" t="s">
-        <v>307</v>
-      </c>
       <c r="D14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2860,19 +2858,19 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" t="s">
+        <v>302</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
         <v>306</v>
-      </c>
-      <c r="C15" t="s">
-        <v>307</v>
-      </c>
-      <c r="D15" t="s">
-        <v>304</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2897,7 +2895,7 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>22</v>
@@ -2941,9 +2939,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2952,8 +2947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2995,7 +2990,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>324</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -3065,7 +3060,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>78</v>
@@ -3101,13 +3096,13 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -3119,13 +3114,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -3137,19 +3132,19 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3240,13 +3235,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -3274,13 +3269,13 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -3291,19 +3286,19 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" t="s">
         <v>313</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" t="s">
-        <v>315</v>
-      </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3311,13 +3306,13 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
@@ -3328,13 +3323,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -3345,13 +3340,13 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -3379,13 +3374,13 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C24" t="s">
         <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -3396,16 +3391,16 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F25" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3413,19 +3408,19 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3447,7 +3442,7 @@
         <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>16</v>
@@ -3464,13 +3459,13 @@
         <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -3478,16 +3473,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
@@ -3495,7 +3490,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
         <v>22</v>
@@ -3512,16 +3507,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -3529,16 +3524,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C33" t="s">
         <v>78</v>
       </c>
       <c r="D33" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -3546,44 +3541,44 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D34" t="s">
+        <v>331</v>
+      </c>
+      <c r="F34" t="s">
         <v>334</v>
-      </c>
-      <c r="F34" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
@@ -3597,10 +3592,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>16</v>
@@ -3614,16 +3609,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B38" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D38" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E38" t="s">
         <v>4</v>
@@ -3631,16 +3626,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B39" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E39" t="s">
         <v>4</v>
@@ -3648,10 +3643,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>22</v>
@@ -3665,16 +3660,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B41" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D41" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E41" t="s">
         <v>4</v>
@@ -3683,7 +3678,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
@@ -3700,10 +3695,10 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>22</v>
@@ -3717,7 +3712,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B44" t="s">
         <v>36</v>
@@ -3734,7 +3729,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B45" t="s">
         <v>24</v>
@@ -3750,9 +3745,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3762,7 +3754,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3803,7 +3795,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>324</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -3873,7 +3865,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>78</v>
@@ -3909,13 +3901,13 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -3927,13 +3919,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -3945,19 +3937,19 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4051,13 +4043,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -4085,22 +4077,19 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C18" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D18" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4110,7 +4099,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4152,7 +4141,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>324</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -4222,7 +4211,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>78</v>
@@ -4258,13 +4247,13 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -4276,13 +4265,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -4294,19 +4283,19 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4383,7 +4372,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>78</v>
@@ -4400,7 +4389,7 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
@@ -4434,13 +4423,13 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -4452,13 +4441,13 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
@@ -4469,13 +4458,13 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
@@ -4489,19 +4478,19 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
+        <v>349</v>
+      </c>
+      <c r="D21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
         <v>352</v>
-      </c>
-      <c r="D21" t="s">
-        <v>353</v>
-      </c>
-      <c r="E21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -4509,13 +4498,13 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -4526,7 +4515,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>22</v>
@@ -4543,10 +4532,10 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D24" t="s">
         <v>88</v>
@@ -4560,10 +4549,10 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D25" t="s">
         <v>94</v>
@@ -4594,13 +4583,13 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -4612,13 +4601,13 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -4629,7 +4618,7 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>22</v>
@@ -4646,33 +4635,33 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C30" t="s">
+        <v>349</v>
+      </c>
+      <c r="D30" t="s">
+        <v>350</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
         <v>352</v>
-      </c>
-      <c r="D30" t="s">
-        <v>353</v>
-      </c>
-      <c r="E30" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -4680,10 +4669,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>22</v>
@@ -4697,13 +4686,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D33" t="s">
         <v>88</v>
@@ -4714,13 +4703,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D34" t="s">
         <v>94</v>
@@ -4731,10 +4720,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>22</v>
@@ -4748,7 +4737,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -4765,10 +4754,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>22</v>
@@ -4782,7 +4771,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -4799,7 +4788,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -4815,9 +4804,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4827,7 +4813,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4868,7 +4854,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>119</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -4938,7 +4924,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>78</v>
@@ -4974,13 +4960,13 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -4992,13 +4978,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -5010,19 +4996,19 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5099,7 +5085,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>78</v>
@@ -5116,7 +5102,7 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>22</v>
@@ -5133,16 +5119,16 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5167,7 +5153,7 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>22</v>
@@ -5214,9 +5200,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5226,7 +5209,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5269,8 +5252,8 @@
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>123</v>
+      <c r="D2" s="7" t="s">
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -5358,7 +5341,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -5420,9 +5403,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5431,8 +5411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5474,7 +5454,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -5562,7 +5542,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -5598,7 +5578,7 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>22</v>
@@ -5615,13 +5595,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -5633,37 +5613,39 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
+        <v>367</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>366</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5671,10 +5653,10 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -5685,16 +5667,16 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5893,7 +5875,7 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>22</v>
@@ -5940,9 +5922,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5952,7 +5931,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5995,7 +5974,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -6082,7 +6061,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -6118,13 +6097,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -6136,13 +6115,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -6154,19 +6133,19 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6243,10 +6222,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -6510,7 +6489,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -6527,7 +6506,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -6544,7 +6523,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>108</v>
@@ -6561,7 +6540,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
@@ -6578,10 +6557,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>78</v>
@@ -6594,9 +6573,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6606,7 +6582,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6649,7 +6625,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -6736,7 +6712,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -6772,13 +6748,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -6790,13 +6766,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -6808,19 +6784,19 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6880,7 +6856,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>16</v>
@@ -6897,10 +6873,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -6911,19 +6887,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -6937,7 +6913,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -6965,19 +6941,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -6985,13 +6961,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -7002,19 +6978,19 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -7028,7 +7004,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -7056,19 +7032,19 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -7076,13 +7052,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -7093,19 +7069,19 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7119,7 +7095,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -7147,24 +7123,24 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -7181,7 +7157,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -7198,7 +7174,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>108</v>
@@ -7215,7 +7191,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
@@ -7232,10 +7208,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>78</v>
@@ -7248,9 +7224,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7259,8 +7232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7303,7 +7276,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -7390,7 +7363,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -7426,13 +7399,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -7444,13 +7417,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -7462,19 +7435,19 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -7534,7 +7507,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>16</v>
@@ -7551,13 +7524,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -7568,19 +7541,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7594,7 +7567,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -7622,19 +7595,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -7659,13 +7632,13 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -7676,19 +7649,19 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -7702,7 +7675,7 @@
         <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -7730,19 +7703,19 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7750,13 +7723,13 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -7767,19 +7740,19 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7793,7 +7766,7 @@
         <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
@@ -7818,36 +7791,36 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
       </c>
       <c r="F31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -7855,27 +7828,27 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>77</v>
@@ -7884,7 +7857,7 @@
         <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -7892,7 +7865,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
         <v>108</v>
@@ -7909,24 +7882,24 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -7943,7 +7916,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -7960,7 +7933,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
         <v>108</v>
@@ -7977,7 +7950,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
@@ -7994,10 +7967,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>78</v>
@@ -8010,9 +7983,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8021,8 +7991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8064,7 +8034,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -8151,7 +8121,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -8187,13 +8157,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -8205,13 +8175,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -8223,19 +8193,19 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -8295,7 +8265,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>16</v>
@@ -8312,13 +8282,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -8329,19 +8299,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -8355,7 +8325,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -8366,19 +8336,19 @@
         <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -8403,13 +8373,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -8420,19 +8390,19 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -8446,7 +8416,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -8474,19 +8444,19 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -8494,13 +8464,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -8511,19 +8481,19 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -8537,7 +8507,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -8565,33 +8535,33 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -8599,27 +8569,27 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>77</v>
@@ -8628,7 +8598,7 @@
         <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -8636,7 +8606,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>108</v>
@@ -8653,24 +8623,24 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -8687,7 +8657,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -8704,7 +8674,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
         <v>108</v>
@@ -8721,7 +8691,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
         <v>36</v>
@@ -8738,10 +8708,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>78</v>
@@ -8754,9 +8724,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8765,8 +8732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8808,7 +8775,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -8895,7 +8862,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -8931,13 +8898,13 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -8949,13 +8916,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -8967,19 +8934,19 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -9039,7 +9006,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>16</v>
@@ -9056,13 +9023,13 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
@@ -9073,19 +9040,19 @@
         <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -9099,7 +9066,7 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
@@ -9127,19 +9094,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -9147,13 +9114,13 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -9164,19 +9131,19 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -9190,7 +9157,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
@@ -9218,19 +9185,19 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -9238,13 +9205,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -9255,19 +9222,19 @@
         <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -9281,7 +9248,7 @@
         <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
@@ -9309,33 +9276,33 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
@@ -9343,27 +9310,27 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>77</v>
@@ -9372,7 +9339,7 @@
         <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
@@ -9380,7 +9347,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>108</v>
@@ -9397,36 +9364,36 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E35" t="s">
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E36" t="s">
         <v>4</v>
@@ -9434,27 +9401,27 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E37" t="s">
         <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
         <v>77</v>
@@ -9463,7 +9430,7 @@
         <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E38" t="s">
         <v>4</v>
@@ -9471,7 +9438,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
         <v>108</v>
@@ -9488,36 +9455,36 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E40" t="s">
         <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E41" t="s">
         <v>4</v>
@@ -9525,27 +9492,27 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E42" t="s">
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B43" t="s">
         <v>77</v>
@@ -9554,7 +9521,7 @@
         <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
@@ -9562,7 +9529,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B44" t="s">
         <v>108</v>
@@ -9579,36 +9546,36 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D45" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E45" t="s">
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E46" t="s">
         <v>4</v>
@@ -9616,27 +9583,27 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B47" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D47" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E47" t="s">
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B48" t="s">
         <v>77</v>
@@ -9645,7 +9612,7 @@
         <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E48" t="s">
         <v>4</v>
@@ -9653,7 +9620,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s">
         <v>108</v>
@@ -9670,27 +9637,27 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E50" t="s">
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B51" t="s">
         <v>35</v>
@@ -9707,7 +9674,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -9724,7 +9691,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B53" t="s">
         <v>108</v>
@@ -9741,7 +9708,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B54" t="s">
         <v>36</v>
@@ -9758,10 +9725,10 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>78</v>
@@ -9774,9 +9741,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9786,7 +9750,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9829,7 +9793,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>119</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -9916,7 +9880,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>78</v>
@@ -9952,7 +9916,7 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>22</v>
@@ -9969,13 +9933,13 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -9987,13 +9951,13 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -10005,19 +9969,19 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -10059,7 +10023,7 @@
         <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>78</v>
@@ -10076,10 +10040,10 @@
         <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D16" t="s">
         <v>111</v>
@@ -10107,7 +10071,7 @@
         <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>16</v>
@@ -10181,7 +10145,7 @@
         <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -10206,10 +10170,10 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D24" t="s">
         <v>111</v>
@@ -10229,7 +10193,7 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
@@ -10246,7 +10210,7 @@
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -10263,7 +10227,7 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -10319,7 +10283,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B31" t="s">
         <v>36</v>
@@ -10336,7 +10300,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -10352,9 +10316,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>